<commit_message>
added submissions to github - marked completed tabs green
</commit_message>
<xml_diff>
--- a/resubmission/resubmission.xlsx
+++ b/resubmission/resubmission.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="23460" tabRatio="978" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ab comments" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="611">
   <si>
     <t>If you refer to UML classes, or more general, to model elements outside of the Archetype Specification and Model, then you should show them with qualified names (or alternatively with a "(from XYZ)" indicator below the class name. [in my oppinion: a qualified name like "UML::Class" is preferrable becuse of its clarity].</t>
   </si>
@@ -1884,9 +1884,6 @@
   </si>
   <si>
     <t>Represents an absolute point in time, as measured on the Gregorian calendar, and specified only to the day.</t>
-  </si>
-  <si>
-    <t>C-DATE</t>
   </si>
   <si>
     <t>ISO 8601-compatible constraint on instances of Date in the form either of a set of
@@ -2425,12 +2422,21 @@
   <si>
     <t>AB46</t>
   </si>
+  <si>
+    <t>Issue entered in github</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>C_DATE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2480,6 +2486,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2498,14 +2511,312 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="303">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2532,12 +2843,326 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="303">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2808,7 +3433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2831,7 +3456,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>49</v>
@@ -2840,7 +3465,7 @@
         <v>50</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E1" t="s">
         <v>51</v>
@@ -2851,12 +3476,12 @@
         <v>94</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="56">
       <c r="A4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -2870,7 +3495,7 @@
     </row>
     <row r="5" spans="1:5" ht="56">
       <c r="A5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -2884,7 +3509,7 @@
     </row>
     <row r="6" spans="1:5" ht="112">
       <c r="A6" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -2898,7 +3523,7 @@
     </row>
     <row r="7" spans="1:5" ht="28">
       <c r="A7" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -2912,7 +3537,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -2926,7 +3551,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -2940,7 +3565,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
@@ -2954,7 +3579,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
@@ -2968,7 +3593,7 @@
     </row>
     <row r="12" spans="1:5" ht="42">
       <c r="A12" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -2982,7 +3607,7 @@
     </row>
     <row r="13" spans="1:5" ht="196">
       <c r="A13" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -2996,7 +3621,7 @@
     </row>
     <row r="14" spans="1:5" ht="42">
       <c r="A14" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
@@ -3010,7 +3635,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
@@ -3024,7 +3649,7 @@
     </row>
     <row r="16" spans="1:5" ht="154">
       <c r="A16" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>12</v>
@@ -3038,7 +3663,7 @@
     </row>
     <row r="17" spans="1:4" ht="70">
       <c r="A17" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
@@ -3052,7 +3677,7 @@
     </row>
     <row r="18" spans="1:4" ht="112">
       <c r="A18" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
@@ -3066,7 +3691,7 @@
     </row>
     <row r="19" spans="1:4" ht="70">
       <c r="A19" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>15</v>
@@ -3080,7 +3705,7 @@
     </row>
     <row r="20" spans="1:4" ht="42">
       <c r="A20" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>16</v>
@@ -3094,7 +3719,7 @@
     </row>
     <row r="21" spans="1:4" ht="56">
       <c r="A21" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
@@ -3108,7 +3733,7 @@
     </row>
     <row r="22" spans="1:4" ht="70">
       <c r="A22" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>18</v>
@@ -3122,7 +3747,7 @@
     </row>
     <row r="23" spans="1:4" ht="56">
       <c r="A23" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>19</v>
@@ -3136,7 +3761,7 @@
     </row>
     <row r="24" spans="1:4" ht="42">
       <c r="A24" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -3150,7 +3775,7 @@
     </row>
     <row r="25" spans="1:4" ht="56">
       <c r="A25" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -3164,7 +3789,7 @@
     </row>
     <row r="26" spans="1:4" ht="70">
       <c r="A26" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>22</v>
@@ -3178,7 +3803,7 @@
     </row>
     <row r="27" spans="1:4" ht="56">
       <c r="A27" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
@@ -3192,7 +3817,7 @@
     </row>
     <row r="28" spans="1:4" ht="70">
       <c r="A28" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
@@ -3206,7 +3831,7 @@
     </row>
     <row r="29" spans="1:4" ht="84">
       <c r="A29" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
@@ -3220,7 +3845,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>27</v>
@@ -3234,7 +3859,7 @@
     </row>
     <row r="31" spans="1:4" ht="56">
       <c r="A31" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>28</v>
@@ -3248,7 +3873,7 @@
     </row>
     <row r="32" spans="1:4" ht="56">
       <c r="A32" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>29</v>
@@ -3262,7 +3887,7 @@
     </row>
     <row r="33" spans="1:4" ht="42">
       <c r="A33" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>30</v>
@@ -3276,7 +3901,7 @@
     </row>
     <row r="34" spans="1:4" ht="28">
       <c r="A34" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>31</v>
@@ -3290,7 +3915,7 @@
     </row>
     <row r="35" spans="1:4" ht="70">
       <c r="A35" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>32</v>
@@ -3304,7 +3929,7 @@
     </row>
     <row r="36" spans="1:4" ht="70">
       <c r="A36" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>33</v>
@@ -3318,7 +3943,7 @@
     </row>
     <row r="37" spans="1:4" ht="42">
       <c r="A37" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>34</v>
@@ -3332,7 +3957,7 @@
     </row>
     <row r="38" spans="1:4" ht="28">
       <c r="A38" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>35</v>
@@ -3346,7 +3971,7 @@
     </row>
     <row r="39" spans="1:4" ht="28">
       <c r="A39" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>36</v>
@@ -3360,7 +3985,7 @@
     </row>
     <row r="40" spans="1:4" ht="42">
       <c r="A40" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>37</v>
@@ -3374,7 +3999,7 @@
     </row>
     <row r="41" spans="1:4" ht="28">
       <c r="A41" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>38</v>
@@ -3388,7 +4013,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>39</v>
@@ -3402,7 +4027,7 @@
     </row>
     <row r="43" spans="1:4" ht="28">
       <c r="A43" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>40</v>
@@ -3416,7 +4041,7 @@
     </row>
     <row r="44" spans="1:4" ht="238">
       <c r="A44" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>41</v>
@@ -3430,7 +4055,7 @@
     </row>
     <row r="45" spans="1:4" ht="56">
       <c r="A45" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>42</v>
@@ -3444,7 +4069,7 @@
     </row>
     <row r="46" spans="1:4" ht="28">
       <c r="A46" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>43</v>
@@ -3458,7 +4083,7 @@
     </row>
     <row r="47" spans="1:4" ht="28">
       <c r="A47" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>44</v>
@@ -3472,7 +4097,7 @@
     </row>
     <row r="48" spans="1:4" ht="42">
       <c r="A48" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>45</v>
@@ -3486,7 +4111,7 @@
     </row>
     <row r="49" spans="1:4" ht="70">
       <c r="A49" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>46</v>
@@ -3500,7 +4125,7 @@
     </row>
     <row r="50" spans="1:4" ht="84">
       <c r="A50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>47</v>
@@ -3526,202 +4151,248 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FF660066"/>
+    <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="149.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="105.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="D1" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="182">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:5" ht="42">
+      <c r="A1" s="15" t="s">
+        <v>608</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="224">
+      <c r="A2" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5">
+      <c r="B4" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>462</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="84">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" ht="98">
+      <c r="A5" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>610</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="D5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="84">
+      <c r="A6" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="84">
-      <c r="A6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" t="s">
         <v>468</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="D6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="126">
+      <c r="A7" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="112">
-      <c r="A7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" t="s">
         <v>472</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="D7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="112">
+      <c r="A8" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="98">
-      <c r="A8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" t="s">
         <v>476</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="224">
+      <c r="A9" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="168">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="112">
+      <c r="A10" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="126">
+      <c r="A11" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="56">
+      <c r="A12" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="70">
-      <c r="A10" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="98">
-      <c r="A11" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="56">
-      <c r="A12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="56">
+      <c r="A13" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="42">
-      <c r="A13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="D13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="42">
+      <c r="A14" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="42">
-      <c r="A14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="D14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="84">
+      <c r="A15" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="70">
-      <c r="A15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="D15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="168">
+      <c r="A16" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="154">
-      <c r="A16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="182">
+      <c r="A17" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="154">
-      <c r="A17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>553</v>
+      <c r="E17" s="1" t="s">
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -3750,7 +4421,7 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="D2" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="78">
@@ -3758,63 +4429,63 @@
         <v>94</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="39">
       <c r="B4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="65">
       <c r="B5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="143">
       <c r="B6" t="s">
+        <v>532</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>533</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="26">
       <c r="B7" t="s">
+        <v>538</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>539</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="42">
       <c r="B8" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="39">
       <c r="B9" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="28">
       <c r="B10" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -3841,7 +4512,7 @@
   <dimension ref="B1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4227,7 +4898,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="E1" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="84">
@@ -4235,7 +4906,7 @@
         <v>94</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5266,103 +5937,135 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FF660066"/>
+    <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="B1:D13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="183.1640625" customWidth="1"/>
+    <col min="4" max="4" width="95.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="1:4" ht="42">
+      <c r="A1" s="14" t="s">
+        <v>608</v>
+      </c>
       <c r="D1" s="8" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" ht="70">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="126">
+      <c r="A2" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B2" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="10" customFormat="1" ht="112">
+      <c r="A4" s="13" t="s">
+        <v>609</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" ht="84">
-      <c r="B4" t="s">
-        <v>513</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="11" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="84">
+      <c r="A5" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B5" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" ht="56">
-      <c r="B5" t="s">
+      <c r="D5" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="D5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="154">
+      <c r="A6" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B6" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" ht="98">
-      <c r="B6" t="s">
+      <c r="D6" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="D6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="56">
+      <c r="A7" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B7" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" ht="42">
-      <c r="B7" t="s">
+      <c r="D7" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="D7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="112">
+      <c r="A8" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B8" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="70">
-      <c r="B8" t="s">
+      <c r="D8" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="56">
+      <c r="A9" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B9" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="28">
-      <c r="B9" t="s">
+      <c r="D9" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="98">
+      <c r="A11" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B11" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" ht="56">
-      <c r="B11" t="s">
+      <c r="D11" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="28">
+    </row>
+    <row r="12" spans="1:4" ht="56">
+      <c r="A12" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B12" t="s">
+        <v>546</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="D12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="28">
+      <c r="A13" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B13" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" t="s">
+      <c r="D13" s="1" t="s">
         <v>549</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -5379,26 +6082,31 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FF660066"/>
+    <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="B1:D7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
-    <col min="4" max="4" width="125.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="4" max="4" width="89.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="1:4" ht="42">
+      <c r="A1" s="14" t="s">
+        <v>608</v>
+      </c>
       <c r="D1" s="7" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" ht="70">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="84">
+      <c r="A2" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B2" t="s">
         <v>94</v>
       </c>
@@ -5406,7 +6114,10 @@
         <v>459</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="56">
+    <row r="3" spans="1:4" ht="84">
+      <c r="A3" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B3" t="s">
         <v>132</v>
       </c>
@@ -5414,7 +6125,10 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="1:4">
+      <c r="A4" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B4" t="s">
         <v>448</v>
       </c>
@@ -5422,7 +6136,10 @@
         <v>449</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="56">
+    <row r="5" spans="1:4" ht="70">
+      <c r="A5" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B5" t="s">
         <v>450</v>
       </c>
@@ -5430,15 +6147,21 @@
         <v>451</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="42">
+    <row r="6" spans="1:4" ht="56">
+      <c r="A6" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B6" t="s">
         <v>452</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="70">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="98">
+      <c r="A7" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B7" t="s">
         <v>457</v>
       </c>
@@ -5448,6 +6171,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5459,26 +6183,31 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FF660066"/>
+    <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="B1:D5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.83203125" customWidth="1"/>
-    <col min="4" max="4" width="112.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="85.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="1:4" ht="42">
+      <c r="A1" s="14" t="s">
+        <v>608</v>
+      </c>
       <c r="D1" s="7" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" ht="70">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="84">
+      <c r="A2" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B2" t="s">
         <v>94</v>
       </c>
@@ -5486,7 +6215,10 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="70">
+    <row r="3" spans="1:4" ht="84">
+      <c r="A3" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B3" t="s">
         <v>132</v>
       </c>
@@ -5494,7 +6226,10 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="56">
+    <row r="4" spans="1:4" ht="84">
+      <c r="A4" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B4" t="s">
         <v>453</v>
       </c>
@@ -5502,7 +6237,10 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="42">
+    <row r="5" spans="1:4" ht="42">
+      <c r="A5" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B5" t="s">
         <v>454</v>
       </c>
@@ -5524,43 +6262,52 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FF660066"/>
+    <tabColor rgb="FF008000"/>
   </sheetPr>
-  <dimension ref="B1:D4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="42.33203125" customWidth="1"/>
-    <col min="4" max="4" width="126.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="98" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="1:4" ht="42">
+      <c r="A1" s="14" t="s">
+        <v>608</v>
+      </c>
       <c r="D1" s="9" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" ht="28">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28">
+      <c r="A2" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B2" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="42">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="56">
+      <c r="A4" s="12" t="s">
+        <v>609</v>
+      </c>
       <c r="B4" t="s">
+        <v>513</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>514</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>515</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5652,18 +6399,18 @@
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="14" spans="2:4">
@@ -5800,10 +6547,10 @@
     </row>
     <row r="38" spans="2:4" ht="84">
       <c r="B38" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -5842,10 +6589,10 @@
     </row>
     <row r="47" spans="2:4" ht="42">
       <c r="B47" t="s">
+        <v>486</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>